<commit_message>
round Diff (MW) values to 2 decimals for display and update difference calculation to round to 2 decimals
</commit_message>
<xml_diff>
--- a/data/january/ins.xlsx
+++ b/data/january/ins.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t xml:space="preserve">S.No</t>
   </si>
@@ -377,10 +377,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4:F100"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -429,6 +429,7 @@
       <c r="F2" s="6" t="n">
         <v>1</v>
       </c>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
@@ -449,71 +450,136 @@
       <c r="F3" s="6" t="n">
         <v>0.0208333333333333</v>
       </c>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>46024</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>0.0729166666666667</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>46024</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>46024</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>46024</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>46025</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>46025</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>0.138888888888889</v>
+      </c>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>46025</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>46025</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>0.572916666666667</v>
+      </c>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>46025</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>0.84375</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>46025</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>0.861111111111111</v>
+      </c>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>46025</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>0.920138888888889</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>46025</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
-        <v>9</v>
-      </c>
+      <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
@@ -521,9 +587,7 @@
       <c r="F10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
-        <v>10</v>
-      </c>
+      <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
@@ -531,9 +595,7 @@
       <c r="F11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
-        <v>11</v>
-      </c>
+      <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
@@ -541,9 +603,7 @@
       <c r="F12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
-        <v>12</v>
-      </c>
+      <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
@@ -551,9 +611,7 @@
       <c r="F13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
-        <v>13</v>
-      </c>
+      <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
@@ -561,9 +619,7 @@
       <c r="F14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
-        <v>14</v>
-      </c>
+      <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
@@ -571,9 +627,7 @@
       <c r="F15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
-        <v>15</v>
-      </c>
+      <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
@@ -581,9 +635,7 @@
       <c r="F16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
-        <v>16</v>
-      </c>
+      <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
@@ -591,9 +643,7 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
-        <v>17</v>
-      </c>
+      <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
@@ -601,9 +651,7 @@
       <c r="F18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
-        <v>18</v>
-      </c>
+      <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -611,9 +659,7 @@
       <c r="F19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
-        <v>19</v>
-      </c>
+      <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -621,9 +667,7 @@
       <c r="F20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
-        <v>20</v>
-      </c>
+      <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -631,9 +675,7 @@
       <c r="F21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
-        <v>21</v>
-      </c>
+      <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
@@ -641,9 +683,7 @@
       <c r="F22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
-        <v>22</v>
-      </c>
+      <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
@@ -651,9 +691,7 @@
       <c r="F23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
-        <v>23</v>
-      </c>
+      <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
@@ -661,9 +699,7 @@
       <c r="F24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
-        <v>24</v>
-      </c>
+      <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
@@ -671,9 +707,7 @@
       <c r="F25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
-        <v>25</v>
-      </c>
+      <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
@@ -681,9 +715,7 @@
       <c r="F26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
-        <v>26</v>
-      </c>
+      <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
@@ -691,9 +723,7 @@
       <c r="F27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="n">
-        <v>27</v>
-      </c>
+      <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
@@ -701,9 +731,7 @@
       <c r="F28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
-        <v>28</v>
-      </c>
+      <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
@@ -711,9 +739,7 @@
       <c r="F29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="n">
-        <v>29</v>
-      </c>
+      <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
@@ -721,9 +747,7 @@
       <c r="F30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="n">
-        <v>30</v>
-      </c>
+      <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
@@ -731,9 +755,7 @@
       <c r="F31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="n">
-        <v>31</v>
-      </c>
+      <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
@@ -741,9 +763,7 @@
       <c r="F32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="n">
-        <v>32</v>
-      </c>
+      <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
@@ -751,9 +771,7 @@
       <c r="F33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="n">
-        <v>33</v>
-      </c>
+      <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
@@ -761,9 +779,7 @@
       <c r="F34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="n">
-        <v>34</v>
-      </c>
+      <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
@@ -771,9 +787,7 @@
       <c r="F35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="n">
-        <v>35</v>
-      </c>
+      <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
@@ -781,9 +795,7 @@
       <c r="F36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="n">
-        <v>36</v>
-      </c>
+      <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
       <c r="D37" s="6"/>
@@ -791,9 +803,7 @@
       <c r="F37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="n">
-        <v>37</v>
-      </c>
+      <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
@@ -801,9 +811,7 @@
       <c r="F38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="n">
-        <v>38</v>
-      </c>
+      <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
@@ -811,9 +819,7 @@
       <c r="F39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="n">
-        <v>39</v>
-      </c>
+      <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
       <c r="D40" s="6"/>
@@ -821,9 +827,7 @@
       <c r="F40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="n">
-        <v>40</v>
-      </c>
+      <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
@@ -831,9 +835,7 @@
       <c r="F41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="n">
-        <v>41</v>
-      </c>
+      <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="5"/>
       <c r="D42" s="6"/>
@@ -841,9 +843,7 @@
       <c r="F42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="n">
-        <v>42</v>
-      </c>
+      <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="5"/>
       <c r="D43" s="6"/>
@@ -851,9 +851,7 @@
       <c r="F43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="n">
-        <v>43</v>
-      </c>
+      <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="5"/>
       <c r="D44" s="6"/>
@@ -861,9 +859,7 @@
       <c r="F44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="n">
-        <v>44</v>
-      </c>
+      <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
@@ -871,9 +867,7 @@
       <c r="F45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="n">
-        <v>45</v>
-      </c>
+      <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="5"/>
       <c r="D46" s="6"/>
@@ -881,9 +875,7 @@
       <c r="F46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="n">
-        <v>46</v>
-      </c>
+      <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="5"/>
       <c r="D47" s="6"/>
@@ -891,9 +883,7 @@
       <c r="F47" s="6"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="3" t="n">
-        <v>47</v>
-      </c>
+      <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="5"/>
       <c r="D48" s="6"/>
@@ -901,9 +891,7 @@
       <c r="F48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3" t="n">
-        <v>48</v>
-      </c>
+      <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="5"/>
       <c r="D49" s="6"/>
@@ -911,9 +899,7 @@
       <c r="F49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="n">
-        <v>49</v>
-      </c>
+      <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="5"/>
       <c r="D50" s="6"/>
@@ -921,9 +907,7 @@
       <c r="F50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="n">
-        <v>50</v>
-      </c>
+      <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="5"/>
       <c r="D51" s="6"/>
@@ -931,9 +915,7 @@
       <c r="F51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="n">
-        <v>51</v>
-      </c>
+      <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="5"/>
       <c r="D52" s="6"/>
@@ -941,9 +923,7 @@
       <c r="F52" s="6"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="n">
-        <v>52</v>
-      </c>
+      <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="5"/>
       <c r="D53" s="6"/>
@@ -951,9 +931,7 @@
       <c r="F53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="n">
-        <v>53</v>
-      </c>
+      <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="5"/>
       <c r="D54" s="6"/>
@@ -961,9 +939,7 @@
       <c r="F54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3" t="n">
-        <v>54</v>
-      </c>
+      <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="5"/>
       <c r="D55" s="6"/>
@@ -971,9 +947,7 @@
       <c r="F55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="n">
-        <v>55</v>
-      </c>
+      <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="5"/>
       <c r="D56" s="6"/>
@@ -981,9 +955,7 @@
       <c r="F56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="3" t="n">
-        <v>56</v>
-      </c>
+      <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="5"/>
       <c r="D57" s="6"/>
@@ -991,9 +963,7 @@
       <c r="F57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3" t="n">
-        <v>57</v>
-      </c>
+      <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="5"/>
       <c r="D58" s="6"/>
@@ -1001,9 +971,7 @@
       <c r="F58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3" t="n">
-        <v>58</v>
-      </c>
+      <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="5"/>
       <c r="D59" s="6"/>
@@ -1011,9 +979,7 @@
       <c r="F59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3" t="n">
-        <v>59</v>
-      </c>
+      <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="5"/>
       <c r="D60" s="6"/>
@@ -1021,9 +987,7 @@
       <c r="F60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3" t="n">
-        <v>60</v>
-      </c>
+      <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="5"/>
       <c r="D61" s="6"/>
@@ -1031,9 +995,7 @@
       <c r="F61" s="6"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="3" t="n">
-        <v>61</v>
-      </c>
+      <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="5"/>
       <c r="D62" s="6"/>
@@ -1041,9 +1003,7 @@
       <c r="F62" s="6"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3" t="n">
-        <v>62</v>
-      </c>
+      <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="5"/>
       <c r="D63" s="6"/>
@@ -1051,9 +1011,7 @@
       <c r="F63" s="6"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="3" t="n">
-        <v>63</v>
-      </c>
+      <c r="A64" s="3"/>
       <c r="B64" s="7"/>
       <c r="C64" s="5"/>
       <c r="D64" s="6"/>
@@ -1061,9 +1019,7 @@
       <c r="F64" s="6"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3" t="n">
-        <v>64</v>
-      </c>
+      <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="5"/>
       <c r="D65" s="6"/>
@@ -1071,9 +1027,7 @@
       <c r="F65" s="6"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3" t="n">
-        <v>65</v>
-      </c>
+      <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="5"/>
       <c r="D66" s="6"/>
@@ -1081,9 +1035,7 @@
       <c r="F66" s="6"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="3" t="n">
-        <v>66</v>
-      </c>
+      <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="5"/>
       <c r="D67" s="6"/>
@@ -1091,9 +1043,7 @@
       <c r="F67" s="6"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="3" t="n">
-        <v>67</v>
-      </c>
+      <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="5"/>
       <c r="D68" s="6"/>
@@ -1101,9 +1051,7 @@
       <c r="F68" s="6"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="n">
-        <v>68</v>
-      </c>
+      <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="5"/>
       <c r="D69" s="6"/>
@@ -1111,9 +1059,7 @@
       <c r="F69" s="6"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3" t="n">
-        <v>69</v>
-      </c>
+      <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="5"/>
       <c r="D70" s="6"/>
@@ -1121,9 +1067,7 @@
       <c r="F70" s="6"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3" t="n">
-        <v>70</v>
-      </c>
+      <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="5"/>
       <c r="D71" s="6"/>
@@ -1131,9 +1075,7 @@
       <c r="F71" s="6"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="3" t="n">
-        <v>71</v>
-      </c>
+      <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="5"/>
       <c r="D72" s="6"/>
@@ -1141,9 +1083,7 @@
       <c r="F72" s="6"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3" t="n">
-        <v>72</v>
-      </c>
+      <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="5"/>
       <c r="D73" s="6"/>
@@ -1151,9 +1091,7 @@
       <c r="F73" s="6"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="3" t="n">
-        <v>73</v>
-      </c>
+      <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="5"/>
       <c r="D74" s="6"/>
@@ -1161,9 +1099,7 @@
       <c r="F74" s="6"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="3" t="n">
-        <v>74</v>
-      </c>
+      <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="5"/>
       <c r="D75" s="6"/>
@@ -1171,9 +1107,7 @@
       <c r="F75" s="6"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="3" t="n">
-        <v>75</v>
-      </c>
+      <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="5"/>
       <c r="D76" s="6"/>
@@ -1181,9 +1115,7 @@
       <c r="F76" s="6"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3" t="n">
-        <v>76</v>
-      </c>
+      <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="5"/>
       <c r="D77" s="6"/>
@@ -1191,9 +1123,7 @@
       <c r="F77" s="6"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3" t="n">
-        <v>77</v>
-      </c>
+      <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="5"/>
       <c r="D78" s="6"/>
@@ -1201,9 +1131,7 @@
       <c r="F78" s="6"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="n">
-        <v>78</v>
-      </c>
+      <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="5"/>
       <c r="D79" s="6"/>
@@ -1211,9 +1139,7 @@
       <c r="F79" s="6"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3" t="n">
-        <v>79</v>
-      </c>
+      <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="5"/>
       <c r="D80" s="6"/>
@@ -1221,9 +1147,7 @@
       <c r="F80" s="6"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3" t="n">
-        <v>80</v>
-      </c>
+      <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="5"/>
       <c r="D81" s="6"/>
@@ -1231,9 +1155,7 @@
       <c r="F81" s="6"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="3" t="n">
-        <v>81</v>
-      </c>
+      <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="5"/>
       <c r="D82" s="6"/>
@@ -1241,9 +1163,7 @@
       <c r="F82" s="6"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3" t="n">
-        <v>82</v>
-      </c>
+      <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="5"/>
       <c r="D83" s="6"/>
@@ -1251,9 +1171,7 @@
       <c r="F83" s="6"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="3" t="n">
-        <v>83</v>
-      </c>
+      <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="5"/>
       <c r="D84" s="6"/>
@@ -1261,9 +1179,7 @@
       <c r="F84" s="6"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3" t="n">
-        <v>84</v>
-      </c>
+      <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="5"/>
       <c r="D85" s="6"/>
@@ -1271,9 +1187,7 @@
       <c r="F85" s="6"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3" t="n">
-        <v>85</v>
-      </c>
+      <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="5"/>
       <c r="D86" s="6"/>
@@ -1281,9 +1195,7 @@
       <c r="F86" s="6"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3" t="n">
-        <v>86</v>
-      </c>
+      <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="5"/>
       <c r="D87" s="6"/>
@@ -1291,9 +1203,7 @@
       <c r="F87" s="6"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3" t="n">
-        <v>87</v>
-      </c>
+      <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="5"/>
       <c r="D88" s="6"/>
@@ -1301,9 +1211,7 @@
       <c r="F88" s="6"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3" t="n">
-        <v>88</v>
-      </c>
+      <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="5"/>
       <c r="D89" s="6"/>
@@ -1311,9 +1219,7 @@
       <c r="F89" s="6"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="3" t="n">
-        <v>89</v>
-      </c>
+      <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="5"/>
       <c r="D90" s="6"/>
@@ -1321,9 +1227,7 @@
       <c r="F90" s="6"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3" t="n">
-        <v>90</v>
-      </c>
+      <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="5"/>
       <c r="D91" s="6"/>
@@ -1331,9 +1235,7 @@
       <c r="F91" s="6"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3" t="n">
-        <v>91</v>
-      </c>
+      <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="5"/>
       <c r="D92" s="6"/>
@@ -1341,9 +1243,7 @@
       <c r="F92" s="6"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3" t="n">
-        <v>92</v>
-      </c>
+      <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="5"/>
       <c r="D93" s="6"/>
@@ -1351,9 +1251,7 @@
       <c r="F93" s="6"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="3" t="n">
-        <v>93</v>
-      </c>
+      <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="5"/>
       <c r="D94" s="6"/>
@@ -1361,9 +1259,7 @@
       <c r="F94" s="6"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3" t="n">
-        <v>94</v>
-      </c>
+      <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="5"/>
       <c r="D95" s="6"/>
@@ -1371,9 +1267,7 @@
       <c r="F95" s="6"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="3" t="n">
-        <v>95</v>
-      </c>
+      <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="5"/>
       <c r="D96" s="6"/>
@@ -1381,9 +1275,7 @@
       <c r="F96" s="6"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="3" t="n">
-        <v>96</v>
-      </c>
+      <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="5"/>
       <c r="D97" s="6"/>
@@ -1391,9 +1283,7 @@
       <c r="F97" s="6"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="3" t="n">
-        <v>97</v>
-      </c>
+      <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="5"/>
       <c r="D98" s="6"/>
@@ -1401,9 +1291,7 @@
       <c r="F98" s="6"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="3" t="n">
-        <v>98</v>
-      </c>
+      <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="5"/>
       <c r="D99" s="6"/>
@@ -1411,9 +1299,7 @@
       <c r="F99" s="6"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="3" t="n">
-        <v>99</v>
-      </c>
+      <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="5"/>
       <c r="D100" s="6"/>

</xml_diff>

<commit_message>
Update ins.xlsx for January with new data
</commit_message>
<xml_diff>
--- a/data/january/ins.xlsx
+++ b/data/january/ins.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t xml:space="preserve">S.No</t>
   </si>
@@ -380,7 +380,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -453,129 +453,57 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>46024</v>
-      </c>
-      <c r="D4" s="6" t="n">
-        <v>0.0729166666666667</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>46024</v>
-      </c>
-      <c r="F4" s="6" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>46024</v>
-      </c>
-      <c r="D5" s="6" t="n">
-        <v>0.916666666666667</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>46024</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>46025</v>
-      </c>
-      <c r="D6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>46025</v>
-      </c>
-      <c r="F6" s="6" t="n">
-        <v>0.138888888888889</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>46025</v>
-      </c>
-      <c r="D7" s="6" t="n">
-        <v>0.4375</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>46025</v>
-      </c>
-      <c r="F7" s="6" t="n">
-        <v>0.572916666666667</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="5" t="n">
-        <v>46025</v>
-      </c>
-      <c r="D8" s="6" t="n">
-        <v>0.84375</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>46025</v>
-      </c>
-      <c r="F8" s="6" t="n">
-        <v>0.861111111111111</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>46025</v>
-      </c>
-      <c r="D9" s="6" t="n">
-        <v>0.920138888888889</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>46025</v>
-      </c>
-      <c r="F9" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
ramp rate colum formula
</commit_message>
<xml_diff>
--- a/data/january/ins.xlsx
+++ b/data/january/ins.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t xml:space="preserve">S.No</t>
   </si>
@@ -152,7 +152,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -169,27 +169,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -392,7 +380,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -441,7 +429,7 @@
       <c r="F2" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
@@ -462,7 +450,7 @@
       <c r="F3" s="6" t="n">
         <v>0.0208333333333333</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
@@ -483,7 +471,7 @@
       <c r="F4" s="6" t="n">
         <v>0.125</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
@@ -504,7 +492,7 @@
       <c r="F5" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
@@ -525,7 +513,7 @@
       <c r="F6" s="6" t="n">
         <v>0.138888888888889</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
@@ -546,7 +534,7 @@
       <c r="F7" s="6" t="n">
         <v>0.572916666666667</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
@@ -567,7 +555,7 @@
       <c r="F8" s="6" t="n">
         <v>0.861111111111111</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
@@ -588,819 +576,735 @@
       <c r="F9" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="5" t="n">
-        <v>46026</v>
-      </c>
-      <c r="D10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>46026</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>0.118055555555556</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="5" t="n">
-        <v>46026</v>
-      </c>
-      <c r="D11" s="6" t="n">
-        <v>0.154861111111111</v>
-      </c>
-      <c r="E11" s="5" t="n">
-        <v>46026</v>
-      </c>
-      <c r="F11" s="6" t="n">
-        <v>0.177083333333333</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="5" t="n">
-        <v>46026</v>
-      </c>
-      <c r="D12" s="6" t="n">
-        <v>0.538194444444444</v>
-      </c>
-      <c r="E12" s="5" t="n">
-        <v>46026</v>
-      </c>
-      <c r="F12" s="6" t="n">
-        <v>0.583333333333333</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="5" t="n">
-        <v>46026</v>
-      </c>
-      <c r="D13" s="6" t="n">
-        <v>0.913194444444445</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>46026</v>
-      </c>
-      <c r="F13" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="5" t="n">
-        <v>46027</v>
-      </c>
-      <c r="D14" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="5" t="n">
-        <v>46027</v>
-      </c>
-      <c r="F14" s="6" t="n">
-        <v>0.15625</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="5" t="n">
-        <v>46027</v>
-      </c>
-      <c r="D15" s="6" t="n">
-        <v>0.447916666666667</v>
-      </c>
-      <c r="E15" s="5" t="n">
-        <v>46027</v>
-      </c>
-      <c r="F15" s="6" t="n">
-        <v>0.486111111111111</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="5" t="n">
-        <v>46027</v>
-      </c>
-      <c r="D16" s="6" t="n">
-        <v>0.53125</v>
-      </c>
-      <c r="E16" s="5" t="n">
-        <v>46027</v>
-      </c>
-      <c r="F16" s="6" t="n">
-        <v>0.579861111111111</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="7"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="7"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="7"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="7"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="7"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="7"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="7"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="7"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="7"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="7"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="7"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="7"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="7"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="7"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="7"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="7"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="7"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="7"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="7"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="7"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="7"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="7"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="7"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="7"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="7"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="7"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="7"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="7"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="7"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="7"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="7"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="6"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="7"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="7"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="7"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="7"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="7"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="6"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="7"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3"/>
-      <c r="B54" s="8"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="7"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="7"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="7"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="7"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="7"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="7"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="7"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="7"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="6"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="7"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="6"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="7"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="6"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="6"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="7"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="6"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3"/>
-      <c r="B66" s="8"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="7"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="6"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="7"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="6"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3"/>
-      <c r="B68" s="8"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="7"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="6"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3"/>
-      <c r="B69" s="8"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="7"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="6"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3"/>
-      <c r="B70" s="8"/>
-      <c r="C70" s="9"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="9"/>
-      <c r="F70" s="7"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="6"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="9"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="7"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="6"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3"/>
-      <c r="B72" s="8"/>
-      <c r="C72" s="9"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="7"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="6"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3"/>
-      <c r="B73" s="8"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="7"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="6"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3"/>
-      <c r="B74" s="8"/>
-      <c r="C74" s="9"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="7"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="6"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3"/>
-      <c r="B75" s="8"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="7"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="6"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="9"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="9"/>
-      <c r="F76" s="7"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="6"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3"/>
-      <c r="B77" s="8"/>
-      <c r="C77" s="9"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="9"/>
-      <c r="F77" s="7"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="6"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3"/>
-      <c r="B78" s="8"/>
-      <c r="C78" s="9"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="7"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="6"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3"/>
-      <c r="B79" s="8"/>
-      <c r="C79" s="9"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="7"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="6"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3"/>
-      <c r="B80" s="8"/>
-      <c r="C80" s="9"/>
-      <c r="D80" s="7"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="7"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="6"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3"/>
-      <c r="B81" s="8"/>
-      <c r="C81" s="9"/>
-      <c r="D81" s="7"/>
-      <c r="E81" s="9"/>
-      <c r="F81" s="7"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="6"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3"/>
-      <c r="B82" s="8"/>
-      <c r="C82" s="9"/>
-      <c r="D82" s="7"/>
-      <c r="E82" s="9"/>
-      <c r="F82" s="7"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="6"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3"/>
-      <c r="B83" s="8"/>
-      <c r="C83" s="9"/>
-      <c r="D83" s="7"/>
-      <c r="E83" s="9"/>
-      <c r="F83" s="7"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="6"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3"/>
-      <c r="B84" s="8"/>
-      <c r="C84" s="9"/>
-      <c r="D84" s="7"/>
-      <c r="E84" s="9"/>
-      <c r="F84" s="7"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="6"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="9"/>
-      <c r="D85" s="7"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="7"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="6"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3"/>
-      <c r="B86" s="8"/>
-      <c r="C86" s="9"/>
-      <c r="D86" s="7"/>
-      <c r="E86" s="9"/>
-      <c r="F86" s="7"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="6"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3"/>
-      <c r="B87" s="8"/>
-      <c r="C87" s="9"/>
-      <c r="D87" s="7"/>
-      <c r="E87" s="9"/>
-      <c r="F87" s="7"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="6"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3"/>
-      <c r="B88" s="8"/>
-      <c r="C88" s="9"/>
-      <c r="D88" s="7"/>
-      <c r="E88" s="9"/>
-      <c r="F88" s="7"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="6"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3"/>
-      <c r="B89" s="8"/>
-      <c r="C89" s="9"/>
-      <c r="D89" s="7"/>
-      <c r="E89" s="9"/>
-      <c r="F89" s="7"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="6"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3"/>
-      <c r="B90" s="8"/>
-      <c r="C90" s="9"/>
-      <c r="D90" s="7"/>
-      <c r="E90" s="9"/>
-      <c r="F90" s="7"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="6"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3"/>
-      <c r="B91" s="8"/>
-      <c r="C91" s="9"/>
-      <c r="D91" s="7"/>
-      <c r="E91" s="9"/>
-      <c r="F91" s="7"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="6"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3"/>
-      <c r="B92" s="8"/>
-      <c r="C92" s="9"/>
-      <c r="D92" s="7"/>
-      <c r="E92" s="9"/>
-      <c r="F92" s="7"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="6"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3"/>
-      <c r="B93" s="8"/>
-      <c r="C93" s="9"/>
-      <c r="D93" s="7"/>
-      <c r="E93" s="9"/>
-      <c r="F93" s="7"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="6"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3"/>
-      <c r="B94" s="8"/>
-      <c r="C94" s="9"/>
-      <c r="D94" s="7"/>
-      <c r="E94" s="9"/>
-      <c r="F94" s="7"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="6"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3"/>
-      <c r="B95" s="8"/>
-      <c r="C95" s="9"/>
-      <c r="D95" s="7"/>
-      <c r="E95" s="9"/>
-      <c r="F95" s="7"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="6"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3"/>
-      <c r="B96" s="8"/>
-      <c r="C96" s="9"/>
-      <c r="D96" s="7"/>
-      <c r="E96" s="9"/>
-      <c r="F96" s="7"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="6"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3"/>
-      <c r="B97" s="8"/>
-      <c r="C97" s="9"/>
-      <c r="D97" s="7"/>
-      <c r="E97" s="9"/>
-      <c r="F97" s="7"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="6"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3"/>
-      <c r="B98" s="8"/>
-      <c r="C98" s="9"/>
-      <c r="D98" s="7"/>
-      <c r="E98" s="9"/>
-      <c r="F98" s="7"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="6"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3"/>
-      <c r="B99" s="8"/>
-      <c r="C99" s="9"/>
-      <c r="D99" s="7"/>
-      <c r="E99" s="9"/>
-      <c r="F99" s="7"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="6"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3"/>
-      <c r="B100" s="8"/>
-      <c r="C100" s="9"/>
-      <c r="D100" s="7"/>
-      <c r="E100" s="9"/>
-      <c r="F100" s="7"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>